<commit_message>
Add Changes to ppt
Added changes in the ppt and worksheet
</commit_message>
<xml_diff>
--- a/Sunburst_Chart.xlsx
+++ b/Sunburst_Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Wine" sheetId="1" r:id="rId1"/>
@@ -888,66 +888,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="double-dagger"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1114425" y="190500"/>
-          <a:ext cx="85725" cy="133350"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1239,7 +1179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -2425,7 +2365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D153"/>
   <sheetViews>
-    <sheetView topLeftCell="A151" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -4581,6 +4521,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>